<commit_message>
Start working on the junction that combines the filament detectors and that uses the quarter turn fittings
</commit_message>
<xml_diff>
--- a/costing_calculator.xlsx
+++ b/costing_calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t xml:space="preserve">Configuration</t>
   </si>
@@ -103,7 +103,10 @@
     <t xml:space="preserve">boards</t>
   </si>
   <si>
-    <t xml:space="preserve">Limit Switch ?</t>
+    <t xml:space="preserve">HiLetgo 10pcs Micro Limit Switch KW12-3 AC 250V 5A SPDT 1NO 1NC Micro Switch Normally Open Close Limit Switch with Roller Lever Arm Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch</t>
   </si>
   <si>
     <t xml:space="preserve">Arduino Uno R4 Minima</t>
@@ -115,13 +118,19 @@
     <t xml:space="preserve">iexcell 400 Pcs M2 x 4/6/8/10/12/14/16/20 Alloy Steel 12.9 Grade High Tensile Hex Socket Head Cap Screws Bolts Nuts Assortment Kit</t>
   </si>
   <si>
-    <t xml:space="preserve">Kit</t>
+    <t xml:space="preserve">kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MUYI 10 Meters = 32.8 Feet PTFE Teflon Tube OD 4mm ID 2mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">meter</t>
   </si>
   <si>
     <t xml:space="preserve">Aclorol 5V 10A 50W Power Supply 100V-240V AC to DC Adapter 5V 10 amp Switching Converter 5.5x2.1mm Plug for WS2811 WS2812B WS2813 5V LED Strip Pixel Lights</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit</t>
+    <t xml:space="preserve">unit</t>
   </si>
 </sst>
 </file>
@@ -138,6 +147,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,6 +169,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,13 +214,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -245,49 +264,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="51.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -310,7 +330,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -323,24 +343,24 @@
         <f aca="false">C4*D4</f>
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">_xlfn.CEILING.MATH(D4*3/16)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <f aca="false">_xlfn.CEILING.MATH(E4*3/8)</f>
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">SUM(C3:C4)</f>
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="4" t="n">
         <f aca="false">SUM(E3:E4)</f>
         <v>18</v>
       </c>
@@ -354,39 +374,39 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="5" t="n">
         <v>18.88</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -403,16 +423,16 @@
         <f aca="false">_xlfn.CEILING.MATH(G9/D9)</f>
         <v>6</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="5" t="n">
         <f aca="false">C9*H9</f>
         <v>113.28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -425,20 +445,20 @@
         <f aca="false">C5</f>
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="4" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G10/D10)</f>
         <v>1</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="5" t="n">
         <f aca="false">C10*H10</f>
         <v>15.99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="5" t="n">
         <v>7</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -455,16 +475,16 @@
         <f aca="false">G11</f>
         <v>4</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="5" t="n">
         <f aca="false">H11*C11</f>
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="5" t="n">
         <v>14.99</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -481,31 +501,55 @@
         <f aca="false">_xlfn.CEILING.MATH(G12/D12)</f>
         <v>1</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="5" t="n">
         <f aca="false">H12*C12</f>
         <v>14.99</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="5" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <f aca="false">C13/D13</f>
+        <v>0.599</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">2*E5</f>
+        <v>36</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(G13/D13)</f>
+        <v>4</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <f aca="false">H13*C13</f>
+        <v>23.96</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3" t="n">
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <v>20</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="n">
         <f aca="false">C14/D14</f>
         <v>20</v>
       </c>
@@ -517,29 +561,29 @@
         <f aca="false">_xlfn.CEILING.MATH(G14/D14)</f>
         <v>2</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="5" t="n">
         <f aca="false">H14*C14</f>
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3"/>
+    <row r="15" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="n">
+      <c r="B16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="n">
         <v>11.68</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>1</v>
@@ -547,63 +591,95 @@
       <c r="H16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="5" t="n">
         <f aca="false">H16*C16</f>
         <v>11.68</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>17.99</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <f aca="false">C18/D18</f>
+        <v>1.799</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">E5</f>
+        <v>18</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(G18/D18)</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <f aca="false">H18*C18</f>
+        <v>35.98</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <f aca="false">C17/D17</f>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <f aca="false">C19/D19</f>
         <v>20</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <f aca="false">C5</f>
         <v>2</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <f aca="false">G17</f>
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="n">
-        <f aca="false">H17*C17</f>
+      <c r="H19" s="0" t="n">
+        <f aca="false">G19</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <f aca="false">H19*C19</f>
         <v>40</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="3" t="n">
-        <f aca="false">SUM(C9:C17)</f>
-        <v>92.55</v>
-      </c>
-      <c r="I19" s="3" t="n">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="n">
+        <f aca="false">SUM(C9:C19)</f>
+        <v>116.53</v>
+      </c>
+      <c r="I20" s="5" t="n">
         <f aca="false">SUM(I9:I16)</f>
-        <v>223.94</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5"/>
+        <v>247.9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>